<commit_message>
fixed reset widget entries upon row insertion. working on adding a horizontal scrollbar for additional column displays. main2.py is the currently working file main3.py is the test file for horizontal scrollbar
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="2022" sheetId="1" state="visible" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="racks">'Lists(DoNotSelectThis)'!$F$2:$F$5</definedName>
     <definedName name="tables">'Lists(DoNotSelectThis)'!$C$2:$C$5</definedName>
   </definedNames>
-  <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.01"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -466,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:XFD1048576"/>
@@ -704,6 +704,337 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>test month</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>888888</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Executive</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>zooey</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>123123</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>notes dito</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>321321</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Others</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Sound System</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>jbl</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>1000000000</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>notes?</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>test ulit</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Kitchen-related</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Microwave Oven</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>11111</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Chair</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Executive</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>asf</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>PY_VAR0</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Executive</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Kitchen-related</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Microwave Oven</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>month focus line</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Others</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>AirCon</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>month</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>focus</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Kitchen-related</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Rice Cooker</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>trying-out</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>auto set</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Computer</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>AVR / UPS</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>instead of</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>py_var0</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Select Category</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Select Category</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Select Category</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Select Category</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Select Category</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Select Category</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Select Category</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Select Category</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Select Category</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Select Category</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Select Category</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -715,7 +1046,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:XFD1048576"/>
@@ -805,6 +1136,43 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>test month</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>888888</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Executive</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>zooey</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>123123</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>notes dito</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -816,10 +1184,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -875,14 +1243,12 @@
           <t>feb</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
+      <c r="B2" t="n">
+        <v>2024</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>wwqr</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -892,17 +1258,52 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>brabd</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>price</t>
-        </is>
+          <t>brando</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>12378141</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>uhh.. notes?</t>
+          <t>departments pa na dropdown</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>di nagki clear all</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>hahahaha</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Conference</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>pang 2024 na page</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>5555555</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>notes dito</t>
         </is>
       </c>
     </row>
@@ -920,7 +1321,7 @@
   </sheetPr>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -933,8 +1334,8 @@
     <col width="15.42578125" bestFit="1" customWidth="1" style="2" min="6" max="6"/>
     <col width="16.42578125" bestFit="1" customWidth="1" style="2" min="7" max="7"/>
     <col width="12.5703125" bestFit="1" customWidth="1" style="2" min="8" max="8"/>
-    <col width="9.140625" customWidth="1" style="2" min="9" max="10"/>
-    <col width="9.140625" customWidth="1" style="2" min="11" max="16384"/>
+    <col width="9.140625" customWidth="1" style="2" min="9" max="11"/>
+    <col width="9.140625" customWidth="1" style="2" min="12" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="1">

</xml_diff>